<commit_message>
add years 2013,2015 to data, improve processing and estimation scripts to accomodate changes
</commit_message>
<xml_diff>
--- a/goaTrawl/Raw Trawl Data/Invert_Species.xlsx
+++ b/goaTrawl/Raw Trawl Data/Invert_Species.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="0" windowWidth="42780" windowHeight="23800" tabRatio="500"/>
+    <workbookView xWindow="620" yWindow="20" windowWidth="25120" windowHeight="15580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="1426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="1427">
   <si>
     <t>Row Labels</t>
   </si>
@@ -4297,6 +4297,9 @@
   </si>
   <si>
     <t>common name</t>
+  </si>
+  <si>
+    <t>MOST COMMON FISH SPECIES</t>
   </si>
 </sst>
 </file>
@@ -4810,13 +4813,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F1365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37:D37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -4833,6 +4838,9 @@
       </c>
       <c r="E4" t="s">
         <v>1425</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1426</v>
       </c>
     </row>
     <row r="5" spans="2:6">

</xml_diff>